<commit_message>
단위값에 맞추어 임시값 작성 Character - MovementSpd 5.75 -> 575
CharacterAtk
- ThrowCooldown 2 -> 20
- SwingCooldown 1 -> 20
- SwingRad 2.5 -> 1.5
</commit_message>
<xml_diff>
--- a/_GameData/CharacterAtkGameData.xlsx
+++ b/_GameData/CharacterAtkGameData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\224dj\Desktop\테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D89CD516-70DE-4652-8E5F-27589978A857}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0CD825A9-DAA5-4604-92BC-2DA86B033080}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9526177C-9DC7-41F9-8D6B-AE5A96483907}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9F0BE4E4-9430-45CB-9EAE-899E7E5C01B2}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterAtkGameData" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="표 스타일 1" pivot="0" count="4" xr9:uid="{7EE3A00A-5F6F-4933-BD42-33268A490059}">
+    <tableStyle name="표 스타일 1" pivot="0" count="4" xr9:uid="{72B858C2-12BE-4F32-BFCB-A787B786D98B}">
       <tableStyleElement type="wholeTable" dxfId="8"/>
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
@@ -540,72 +540,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{B28AFCD5-D520-45FA-AA1D-5D81679EBB7C}" name="CharacterAtkTable" displayName="CharacterAtkTable" ref="B2:AO3" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{44584B93-D12C-4B02-944A-5A6F83042B44}" name="CharacterAtkTable" displayName="CharacterAtkTable" ref="B2:AO3" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B2:AO3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{EEB31A55-543F-43CB-8BB1-19EA822A5796}" name="Index"/>
-    <tableColumn id="20" xr3:uid="{16C080CB-DED8-41CE-AF4B-31F455A60D5F}" name="#설명" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{034FF2C3-B424-4052-A8A9-B2027F779CB1}" name="ThrowCooldown" dataDxfId="2"/>
-    <tableColumn id="33" xr3:uid="{55468FB1-8F31-4A78-B598-A2B2EE791D40}" name="ThrowAfterDelay" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{71B7CF92-47FA-4B47-BC0C-968D23A05566}" name="ThrowSpd"/>
-    <tableColumn id="31" xr3:uid="{FAB66652-6049-45EF-9322-500E72E17607}" name="ThrowBounceCount"/>
-    <tableColumn id="4" xr3:uid="{A134644B-0F52-4FBE-BBC2-BFBCAF98911A}" name="SwingCooldown" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{3C284DDE-047B-497F-9613-2A2E6AB1E9FF}" name="SwingAfterDelay"/>
-    <tableColumn id="2" xr3:uid="{8ACAFA53-395E-4DC8-B685-11A8CD3665AE}" name="SwingRad"/>
-    <tableColumn id="3" xr3:uid="{922F40A2-487D-4740-90A0-D47D17C800D1}" name="SwingCentralAngle"/>
-    <tableColumn id="8" xr3:uid="{45862E59-BA95-445F-99EA-1178F27090CF}" name="ChargeTime1"/>
-    <tableColumn id="9" xr3:uid="{4F474FE0-6DCF-4FCC-BB75-BDAD3A56E31F}" name="ChargeTime2"/>
-    <tableColumn id="10" xr3:uid="{4C631BA3-0214-470E-9BF5-2E8E153832BE}" name="ChargeTime3"/>
-    <tableColumn id="11" xr3:uid="{F830B60B-1E42-4497-99A7-6736B1302BF6}" name="ChargeAtkPierce"/>
-    <tableColumn id="16" xr3:uid="{6DECE5D2-885A-4CAB-A58E-BB430C2C8731}" name="ChargeShootSpd1"/>
-    <tableColumn id="17" xr3:uid="{E5F03697-4E53-4386-857C-E7D0638EE88A}" name="ChargeShootSpd2"/>
-    <tableColumn id="18" xr3:uid="{DAE5D131-EF7C-490A-9E20-A92D60A16F35}" name="ChargeShootSpd3"/>
-    <tableColumn id="21" xr3:uid="{4497FDF5-3141-4E32-81C9-13370C985A43}" name="ChargeShootSpd4"/>
-    <tableColumn id="22" xr3:uid="{73907395-4581-47E3-B8AA-A0F354AF0990}" name="ChargeBounceCount1"/>
-    <tableColumn id="23" xr3:uid="{700D44E1-4F88-4978-A3DA-956D8C0CC10B}" name="ChargeBounceCount2"/>
-    <tableColumn id="24" xr3:uid="{7D8D4834-9C80-4FCB-AF1B-264F92E3A13D}" name="ChargeBounceCount3"/>
-    <tableColumn id="25" xr3:uid="{C8E6E190-807A-4E06-9628-7F3633AE349F}" name="ChargeBounceCount4"/>
-    <tableColumn id="12" xr3:uid="{5B93D85B-59B3-46C5-B5DE-2037A92F0D27}" name="ChargeRigidDmg1"/>
-    <tableColumn id="13" xr3:uid="{A45DAFF5-D8DD-42A6-A0BC-2EEB0794FE03}" name="ChargeRigidDmg2"/>
-    <tableColumn id="14" xr3:uid="{03E15F36-BD5D-44A8-B5D0-2975F95F806B}" name="ChargeRigidDmg3"/>
-    <tableColumn id="15" xr3:uid="{FB18BBB9-68E2-4D4C-9844-F8039508D366}" name="ChargeRigidDmg4"/>
-    <tableColumn id="26" xr3:uid="{909E4AE5-CA4F-408B-B1E3-7758B36F3A61}" name="ChargeProjectileDmg1"/>
-    <tableColumn id="27" xr3:uid="{9B9C92D1-2429-4662-91D4-16228C26E0E4}" name="ChargeProjectileDmg2"/>
-    <tableColumn id="28" xr3:uid="{22245C3A-B3E6-4266-812C-F7091817F06A}" name="ChargeProjectileDmg3"/>
-    <tableColumn id="29" xr3:uid="{F8666579-C6A6-47B1-AB58-8EABDAB1A53D}" name="ChargeProjectileDmg4"/>
-    <tableColumn id="19" xr3:uid="{B644CAEA-4AD4-43FB-957C-235805BB472E}" name="AtkDmgPer"/>
-    <tableColumn id="5" xr3:uid="{F7AF8A8F-7EC5-4BD5-AE3C-6033EA856371}" name="#던지기 DPS">
+    <tableColumn id="1" xr3:uid="{D7493F92-EDB2-4F1D-91BB-98DA9B1A50D6}" name="Index"/>
+    <tableColumn id="20" xr3:uid="{D0571948-1A6F-4E00-839E-6EC4026F2CA3}" name="#설명" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{24DED517-AEBF-4822-B025-65CA011D7A57}" name="ThrowCooldown" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{423EF83D-0C61-4FB2-AD7E-DEF2D4DC3C7F}" name="ThrowAfterDelay" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{0030A352-AA92-4585-9C3C-34AA022AA412}" name="ThrowSpd"/>
+    <tableColumn id="31" xr3:uid="{BBA608DC-E837-49D5-B366-8A446C05778F}" name="ThrowBounceCount"/>
+    <tableColumn id="4" xr3:uid="{33F25294-A291-4E52-B9C4-B9AC6A494F8E}" name="SwingCooldown" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{0530D865-9119-4D72-979C-A5EFCB197C50}" name="SwingAfterDelay"/>
+    <tableColumn id="2" xr3:uid="{E0930E97-11F7-47EE-9888-2E3F5CFD0F57}" name="SwingRad"/>
+    <tableColumn id="3" xr3:uid="{33B80F41-8810-4E80-B74D-890580FB5BED}" name="SwingCentralAngle"/>
+    <tableColumn id="8" xr3:uid="{098E095B-D36A-454D-A4A4-3368306C3FB8}" name="ChargeTime1"/>
+    <tableColumn id="9" xr3:uid="{E1C60BC4-0806-4BC9-8096-D96096B91F5B}" name="ChargeTime2"/>
+    <tableColumn id="10" xr3:uid="{31A1CF4A-1301-4FE9-A1A3-B08B5E9CF088}" name="ChargeTime3"/>
+    <tableColumn id="11" xr3:uid="{24D5ABAE-0608-4FCE-A9C3-57C09E6DD3A4}" name="ChargeAtkPierce"/>
+    <tableColumn id="16" xr3:uid="{58807052-AA0D-4637-A286-0301AB99624D}" name="ChargeShootSpd1"/>
+    <tableColumn id="17" xr3:uid="{639777C2-5FEC-480A-BC57-5DD091B69EA5}" name="ChargeShootSpd2"/>
+    <tableColumn id="18" xr3:uid="{CD6A4255-3AF0-4D02-A9C9-7806108BA694}" name="ChargeShootSpd3"/>
+    <tableColumn id="21" xr3:uid="{D8FFAA82-0072-4B30-A01A-4A34BB2E2D41}" name="ChargeShootSpd4"/>
+    <tableColumn id="22" xr3:uid="{EF11C1E1-C89C-4AE0-8995-813CFC63FB46}" name="ChargeBounceCount1"/>
+    <tableColumn id="23" xr3:uid="{BAC28BD5-883D-4E38-85F4-CBAB67BA1533}" name="ChargeBounceCount2"/>
+    <tableColumn id="24" xr3:uid="{367D2EB2-BC81-4D22-8BCC-C3DC12953A23}" name="ChargeBounceCount3"/>
+    <tableColumn id="25" xr3:uid="{59F549D1-492E-4597-9618-E2A4A7BBC002}" name="ChargeBounceCount4"/>
+    <tableColumn id="12" xr3:uid="{55AD5EFA-3A8C-4A37-97C0-38DB26AFE063}" name="ChargeRigidDmg1"/>
+    <tableColumn id="13" xr3:uid="{092D58E2-5044-4C7C-B2DB-3C0AC3998993}" name="ChargeRigidDmg2"/>
+    <tableColumn id="14" xr3:uid="{3BC9CC49-E31B-45F3-81D8-F803F931972F}" name="ChargeRigidDmg3"/>
+    <tableColumn id="15" xr3:uid="{8BD417CC-56BD-427D-BFCC-75C779B06FC4}" name="ChargeRigidDmg4"/>
+    <tableColumn id="26" xr3:uid="{C1ACDFE2-66A4-4186-B0AB-689941D74646}" name="ChargeProjectileDmg1"/>
+    <tableColumn id="27" xr3:uid="{DF74424B-0130-4073-987D-57FA7F10E2B3}" name="ChargeProjectileDmg2"/>
+    <tableColumn id="28" xr3:uid="{5324BA43-11EC-485B-9150-980971E3C0F8}" name="ChargeProjectileDmg3"/>
+    <tableColumn id="29" xr3:uid="{0A77478D-B73C-4A2F-9C6A-ED4DEC4ACD74}" name="ChargeProjectileDmg4"/>
+    <tableColumn id="19" xr3:uid="{D1DA91A2-8952-48BC-B4DB-4AC9BF629F66}" name="AtkDmgPer"/>
+    <tableColumn id="5" xr3:uid="{CFB95128-E1E4-444F-8051-D550AB6B1FF7}" name="#던지기 DPS">
       <calculatedColumnFormula>INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0)) /
 ( CharacterAtkTable[[#This Row],[ThrowCooldown]] * (1 + (CharacterAtkTable[[#This Row],[ThrowBounceCount]]/2)) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{B7643A58-A758-4217-AF8C-25E8EE463DB5}" name="#휘두르기 직접 공격 DPS">
+    <tableColumn id="32" xr3:uid="{876B9209-F126-4505-B0FA-02FEF3774953}" name="#휘두르기 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg1]]/CharacterAtkTable[[#This Row],[SwingCooldown]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{1B566AD8-C301-4E67-8DB0-487EBD8DDE76}" name="#차징1 직접 공격 DPS">
+    <tableColumn id="34" xr3:uid="{4B9750A3-4609-4780-A319-F245CB447865}" name="#차징1 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg2]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{BA20B484-8F37-428A-8C7A-7D6EE1FFA6F5}" name="#차징2 직접 공격 DPS">
+    <tableColumn id="35" xr3:uid="{65397134-BA52-446B-836C-EE7346A9AAD6}" name="#차징2 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg3]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{AE50C797-D4C7-4E36-A9D5-33936ADC3C2D}" name="#차징3 직접 공격 DPS">
+    <tableColumn id="36" xr3:uid="{A8057849-DF00-4BBB-8DBF-51E9B9D46544}" name="#차징3 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg4]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime3]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{4B892A8B-E1B9-4564-AB63-A61754C65ACF}" name="#던진공 튕겨내기 DPS">
+    <tableColumn id="37" xr3:uid="{E0E6A719-C36A-46F6-AE0F-45ADC91B2874}" name="#던진공 튕겨내기 DPS">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg1]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] ) + CharacterAtkTable[[#This Row],[ThrowAfterDelay]]
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount1]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{5E6298E1-F39F-48A5-AD08-837380C0B0AE}" name="#던진공 차징1 튕겨내기 DPS">
+    <tableColumn id="38" xr3:uid="{1CDA5305-A973-43E7-8A7C-97AA0FB2721B}" name="#던진공 차징1 튕겨내기 DPS">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg2]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime1]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount2]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{6F962881-EB84-40E2-AD9E-304BB4027FB6}" name="#던진공 차징2 튕겨내기 DPS3">
+    <tableColumn id="39" xr3:uid="{0674B944-F39B-4DD2-91BA-18A5343F1ACA}" name="#던진공 차징2 튕겨내기 DPS3">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg3]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime2]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount3]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{E576287E-5647-4A4A-8C19-948D0FA07F2F}" name="#던진공 차징3 튕겨내기 DPS4">
+    <tableColumn id="40" xr3:uid="{581B10C6-ABF8-4F1D-AA39-3426C9383E3A}" name="#던진공 차징3 튕겨내기 DPS4">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg4]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime3]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount4]]/2))</calculatedColumnFormula>
@@ -911,14 +911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EFDF040-E357-4F80-BD2B-3C51F506F0F2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5277104-5364-4B02-AFC0-4EBA49F1C0E4}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B1:AO3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1176,7 +1176,7 @@
         <v>44</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="E3">
         <v>1.2</v>
@@ -1188,13 +1188,13 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="I3">
         <v>0.5</v>
       </c>
       <c r="J3">
-        <v>2.5</v>
+        <v>1.5</v>
       </c>
       <c r="K3">
         <v>120</v>
@@ -1265,47 +1265,47 @@
       <c r="AG3">
         <f>INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0)) /
 ( CharacterAtkTable[[#This Row],[ThrowCooldown]] * (1 + (CharacterAtkTable[[#This Row],[ThrowBounceCount]]/2)) )</f>
-        <v>12.5</v>
+        <v>1.25</v>
       </c>
       <c r="AH3">
         <f>CharacterAtkTable[[#This Row],[ChargeRigidDmg1]]/CharacterAtkTable[[#This Row],[SwingCooldown]]</f>
-        <v>10</v>
+        <v>0.5</v>
       </c>
       <c r="AI3">
         <f>CharacterAtkTable[[#This Row],[ChargeRigidDmg2]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime1]])</f>
-        <v>10</v>
+        <v>0.73170731707317072</v>
       </c>
       <c r="AJ3">
         <f>CharacterAtkTable[[#This Row],[ChargeRigidDmg3]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime2]])</f>
-        <v>10</v>
+        <v>0.95238095238095233</v>
       </c>
       <c r="AK3">
         <f>CharacterAtkTable[[#This Row],[ChargeRigidDmg4]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime3]])</f>
-        <v>12</v>
+        <v>1.3953488372093024</v>
       </c>
       <c r="AL3">
         <f>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg1]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] ) + CharacterAtkTable[[#This Row],[ThrowAfterDelay]]
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount1]]/2))</f>
-        <v>38</v>
+        <v>4.75</v>
       </c>
       <c r="AM3">
         <f>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg2]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime1]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount2]]/2))</f>
-        <v>37.037037037037031</v>
+        <v>4.6082949308755765</v>
       </c>
       <c r="AN3">
         <f>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg3]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime2]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount3]]/2))</f>
-        <v>42.1875</v>
+        <v>6.0810810810810816</v>
       </c>
       <c r="AO3">
         <f>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg4]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime3]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount4]]/2))</f>
-        <v>52.027027027027025</v>
+        <v>8.4801762114537453</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
EnemyAtkTable -> AimType: 타입 값 명칭 오류 수정 - World (기존 Angle) - Target (기존 PC) - MoveDirection (신규)
</commit_message>
<xml_diff>
--- a/_GameData/CharacterAtkGameData.xlsx
+++ b/_GameData/CharacterAtkGameData.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\224dj\Desktop\테이블\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9BE796A-6743-41BC-A5BE-36E40A0396BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3954F7C4-94DF-4393-9679-061A380FBCC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6CC10F4C-5C91-4C76-928B-44FB2C132F79}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{85CF85C0-0DC2-41E8-93C5-A815DE396A7A}"/>
   </bookViews>
   <sheets>
     <sheet name="CharacterAtkGameData" sheetId="1" r:id="rId1"/>
@@ -475,7 +475,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="표 스타일 1" pivot="0" count="4" xr9:uid="{244457BE-F43A-4D12-B406-CD31E2E37E4B}">
+    <tableStyle name="표 스타일 1" pivot="0" count="4" xr9:uid="{AD8F274E-20AC-4368-86D3-92F43C17BD3B}">
       <tableStyleElement type="wholeTable" dxfId="8"/>
       <tableStyleElement type="headerRow" dxfId="7"/>
       <tableStyleElement type="firstRowStripe" dxfId="6"/>
@@ -540,72 +540,72 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3DF7FF33-FA69-405B-872A-5628024373E3}" name="CharacterAtkTable" displayName="CharacterAtkTable" ref="B2:AO3" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{725CE467-5B28-4A62-BE06-FAEC96F970D4}" name="CharacterAtkTable" displayName="CharacterAtkTable" ref="B2:AO3" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B2:AO3" xr:uid="{00000000-0009-0000-0100-000007000000}"/>
   <tableColumns count="40">
-    <tableColumn id="1" xr3:uid="{F24BB758-0034-4E76-B368-D7EC0AA2693F}" name="Index"/>
-    <tableColumn id="20" xr3:uid="{80A4BF56-75F3-4BFB-892C-F69092C621BD}" name="#설명" dataDxfId="3"/>
-    <tableColumn id="7" xr3:uid="{A9D24405-8323-4649-B7F5-EF1BA84996BE}" name="ThrowCooldown" dataDxfId="2"/>
-    <tableColumn id="33" xr3:uid="{E777F458-C260-4971-8A06-3111FFCF78BF}" name="ThrowAfterDelay" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{CB7F6A0E-FD91-4D13-A2F6-E67023709774}" name="ThrowSpd"/>
-    <tableColumn id="31" xr3:uid="{24D48661-8D6E-4604-BFA0-706D8B84829E}" name="ThrowBounceCount"/>
-    <tableColumn id="4" xr3:uid="{5133EBF6-3A68-4836-BBC0-8F7C50DBE7AB}" name="SwingCooldown" dataDxfId="0"/>
-    <tableColumn id="6" xr3:uid="{85C7F51C-4F1B-43BE-82E1-95CF849226CF}" name="SwingAfterDelay"/>
-    <tableColumn id="2" xr3:uid="{866BAC07-BA18-40CA-9741-7AA80F0DD8D3}" name="SwingRad"/>
-    <tableColumn id="3" xr3:uid="{A9B77715-7B0B-4BF9-A69B-BF59B518D06E}" name="SwingCentralAngle"/>
-    <tableColumn id="8" xr3:uid="{C6BF2D2D-2F95-4C91-BE65-671886DE74A1}" name="ChargeTime1"/>
-    <tableColumn id="9" xr3:uid="{C69378E6-B4C8-45EE-B3F7-F33776BD9A36}" name="ChargeTime2"/>
-    <tableColumn id="10" xr3:uid="{1CD51A9C-5D3D-4023-AE60-0E3D65FA3D7A}" name="ChargeTime3"/>
-    <tableColumn id="11" xr3:uid="{0480E87A-2595-461A-96DC-2A4354CE179A}" name="ChargeAtkPierce"/>
-    <tableColumn id="16" xr3:uid="{69A7179D-18F2-4C4B-834D-1808D1D15A1A}" name="ChargeShootSpd1"/>
-    <tableColumn id="17" xr3:uid="{BE48A954-9D24-4D62-A73B-935230C7F593}" name="ChargeShootSpd2"/>
-    <tableColumn id="18" xr3:uid="{337011C0-A626-4820-B64E-A8314D761267}" name="ChargeShootSpd3"/>
-    <tableColumn id="21" xr3:uid="{C5D9744F-6810-4E70-BF72-C9B6417955FB}" name="ChargeShootSpd4"/>
-    <tableColumn id="22" xr3:uid="{5CCDD876-0D57-4782-B1A5-AE4837C18453}" name="ChargeBounceCount1"/>
-    <tableColumn id="23" xr3:uid="{555F50AB-882C-4920-84B1-076504A60FC9}" name="ChargeBounceCount2"/>
-    <tableColumn id="24" xr3:uid="{777DE44C-F43F-41C5-B197-814799FD54C7}" name="ChargeBounceCount3"/>
-    <tableColumn id="25" xr3:uid="{4FA304A9-27B1-46A9-9820-32382AB8B815}" name="ChargeBounceCount4"/>
-    <tableColumn id="12" xr3:uid="{A5E1169A-CBE7-43D2-A4A2-D99B18B8E2C0}" name="ChargeRigidDmg1"/>
-    <tableColumn id="13" xr3:uid="{18C5D247-72F4-4778-BAB4-08EE0D835D8B}" name="ChargeRigidDmg2"/>
-    <tableColumn id="14" xr3:uid="{1077C84C-8B56-406A-A541-E43EA88CC84C}" name="ChargeRigidDmg3"/>
-    <tableColumn id="15" xr3:uid="{8EE5C586-264F-4D71-8D1B-5068D6C0A1DB}" name="ChargeRigidDmg4"/>
-    <tableColumn id="26" xr3:uid="{5E132289-829E-45EC-B726-ADAA51F989D2}" name="ChargeProjectileDmg1"/>
-    <tableColumn id="27" xr3:uid="{F00C767D-BA01-4358-ACBD-3A265CBBD8E2}" name="ChargeProjectileDmg2"/>
-    <tableColumn id="28" xr3:uid="{A73DF32B-014A-48F2-8047-F481AEA6EC3E}" name="ChargeProjectileDmg3"/>
-    <tableColumn id="29" xr3:uid="{4DA3E613-5688-4EAF-89E7-A688A0A2A15D}" name="ChargeProjectileDmg4"/>
-    <tableColumn id="19" xr3:uid="{43595A75-8EA9-4F3E-9A53-1C29BE5D27BB}" name="AtkDmgPer"/>
-    <tableColumn id="5" xr3:uid="{62CFA133-14A2-4A25-B1FE-9D9D75B50F1C}" name="#던지기 DPS">
+    <tableColumn id="1" xr3:uid="{C1B5F6C8-79BE-469A-82F4-DB602B4EFFFC}" name="Index"/>
+    <tableColumn id="20" xr3:uid="{63AA380A-077E-4638-AB0E-6E39C5C3FEB1}" name="#설명" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{8A2EDE3B-CB12-4720-86F1-4F3253C8B414}" name="ThrowCooldown" dataDxfId="2"/>
+    <tableColumn id="33" xr3:uid="{F27A0CDC-F12F-46F6-9856-2A892F7B14FE}" name="ThrowAfterDelay" dataDxfId="1"/>
+    <tableColumn id="30" xr3:uid="{F9460254-2644-487B-A6A9-708C67BA56FB}" name="ThrowSpd"/>
+    <tableColumn id="31" xr3:uid="{3A2E8C02-1F09-4431-9009-A20D3E3036CE}" name="ThrowBounceCount"/>
+    <tableColumn id="4" xr3:uid="{A4E9A56E-39EE-4873-A774-7E6F2184CBE5}" name="SwingCooldown" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{FCBEFBF5-FB0F-4CCD-8EEB-652B68BAE2B7}" name="SwingAfterDelay"/>
+    <tableColumn id="2" xr3:uid="{4ADCB0BF-530D-495C-B4F3-9DFBCFF1AEE3}" name="SwingRad"/>
+    <tableColumn id="3" xr3:uid="{DED217E8-B8FE-4083-B38E-C31E93235034}" name="SwingCentralAngle"/>
+    <tableColumn id="8" xr3:uid="{5CD40A88-F036-4C44-A276-989118A060D5}" name="ChargeTime1"/>
+    <tableColumn id="9" xr3:uid="{4C18E74E-3FB5-4B69-BB7C-4A4F30BFF61C}" name="ChargeTime2"/>
+    <tableColumn id="10" xr3:uid="{FF45C111-B723-4C46-A694-C7CE766CC41E}" name="ChargeTime3"/>
+    <tableColumn id="11" xr3:uid="{60B625DC-1A5E-4667-9FA2-C7814F8D559E}" name="ChargeAtkPierce"/>
+    <tableColumn id="16" xr3:uid="{7F56CE77-75AA-4438-BC58-AD6CFEA772B7}" name="ChargeShootSpd1"/>
+    <tableColumn id="17" xr3:uid="{F3060BD7-6117-4B21-83A3-F005B2084AE2}" name="ChargeShootSpd2"/>
+    <tableColumn id="18" xr3:uid="{DE542714-878E-45AB-B8A0-8BB169C2A66C}" name="ChargeShootSpd3"/>
+    <tableColumn id="21" xr3:uid="{A84115C7-E5E0-4E16-A229-BE8B51CC220A}" name="ChargeShootSpd4"/>
+    <tableColumn id="22" xr3:uid="{05D58792-7B49-42C8-AA44-3102E514DF18}" name="ChargeBounceCount1"/>
+    <tableColumn id="23" xr3:uid="{E1D1CE7D-4E52-460B-BE3A-4FCFA22A51BA}" name="ChargeBounceCount2"/>
+    <tableColumn id="24" xr3:uid="{DDED6A86-46CC-4892-8D8C-D8013A2FE015}" name="ChargeBounceCount3"/>
+    <tableColumn id="25" xr3:uid="{0FF73232-E17B-46A2-BF37-C1F21530248C}" name="ChargeBounceCount4"/>
+    <tableColumn id="12" xr3:uid="{99CD85AD-5340-462D-ADBE-A509AB729FE1}" name="ChargeRigidDmg1"/>
+    <tableColumn id="13" xr3:uid="{EB2EA11A-F74B-4E76-A3AB-12894BAC55F1}" name="ChargeRigidDmg2"/>
+    <tableColumn id="14" xr3:uid="{D4DDE864-7A53-4570-A3C5-0959DD8AE54A}" name="ChargeRigidDmg3"/>
+    <tableColumn id="15" xr3:uid="{3F83D9F7-1B56-4C4A-B569-6ED2F023478C}" name="ChargeRigidDmg4"/>
+    <tableColumn id="26" xr3:uid="{1F4707B1-2995-4E25-A2BF-A8C0410DB9EE}" name="ChargeProjectileDmg1"/>
+    <tableColumn id="27" xr3:uid="{6F4B57D0-A2B7-4F04-AC7B-E3249A3F9978}" name="ChargeProjectileDmg2"/>
+    <tableColumn id="28" xr3:uid="{88581F90-1901-413D-AAE2-FD927C60140E}" name="ChargeProjectileDmg3"/>
+    <tableColumn id="29" xr3:uid="{AFA947CA-DFDC-42FF-990D-6578FEA4AE6E}" name="ChargeProjectileDmg4"/>
+    <tableColumn id="19" xr3:uid="{9B7CE9CD-D1EF-4FC1-8EA7-5A35E41B502E}" name="AtkDmgPer"/>
+    <tableColumn id="5" xr3:uid="{161C0A91-EB60-4AB2-9C7A-1A6DA634CD4D}" name="#던지기 DPS">
       <calculatedColumnFormula>INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0)) /
 ( CharacterAtkTable[[#This Row],[ThrowCooldown]] * (1 + (CharacterAtkTable[[#This Row],[ThrowBounceCount]]/2)) )</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="32" xr3:uid="{910FC9C2-2DD9-4A48-95B0-CABADC493EBD}" name="#휘두르기 직접 공격 DPS">
+    <tableColumn id="32" xr3:uid="{4C4EFEDE-945B-4B0B-BD96-0404C305A7C7}" name="#휘두르기 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg1]]/CharacterAtkTable[[#This Row],[SwingCooldown]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{4A29F940-F4AE-4744-92FD-5F1B7C525513}" name="#차징1 직접 공격 DPS">
+    <tableColumn id="34" xr3:uid="{427CA408-295E-425D-B48C-13ACD75B11D8}" name="#차징1 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg2]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime1]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="35" xr3:uid="{A24D8213-08B1-4C54-98EC-3D82ED011221}" name="#차징2 직접 공격 DPS">
+    <tableColumn id="35" xr3:uid="{8AB7185F-071D-4AFB-AAAA-BE15F125EC4C}" name="#차징2 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg3]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime2]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="36" xr3:uid="{9025F080-330A-4226-B0C2-CA0F38B9EA4E}" name="#차징3 직접 공격 DPS">
+    <tableColumn id="36" xr3:uid="{ACFD0B8D-E40F-40CA-9500-E6635E1D48AA}" name="#차징3 직접 공격 DPS">
       <calculatedColumnFormula>CharacterAtkTable[[#This Row],[ChargeRigidDmg4]]/(CharacterAtkTable[[#This Row],[SwingCooldown]]+CharacterAtkTable[[#This Row],[ChargeTime3]])</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="37" xr3:uid="{4E0241C2-4909-4486-8F4F-216139948B80}" name="#던진공 튕겨내기 DPS">
+    <tableColumn id="37" xr3:uid="{CF1EB7B7-9A24-44D1-B9FE-183FB81D74A8}" name="#던진공 튕겨내기 DPS">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg1]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] ) + CharacterAtkTable[[#This Row],[ThrowAfterDelay]]
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount1]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="38" xr3:uid="{056D54B2-0DF2-4991-B3CD-434A5DA8E1C0}" name="#던진공 차징1 튕겨내기 DPS">
+    <tableColumn id="38" xr3:uid="{BB8BE7E2-E11E-49E3-BAA6-A43D4C06BF2E}" name="#던진공 차징1 튕겨내기 DPS">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg2]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime1]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount2]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="39" xr3:uid="{982C92C0-516A-4478-A49A-EA655BC79EB9}" name="#던진공 차징2 튕겨내기 DPS3">
+    <tableColumn id="39" xr3:uid="{CC025782-6265-4F6B-BB62-964AE13DC88B}" name="#던진공 차징2 튕겨내기 DPS3">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg3]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime2]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount3]]/2))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="40" xr3:uid="{24C8D47C-3CC8-4F71-AF65-FE6E98B3D9B4}" name="#던진공 차징3 튕겨내기 DPS4">
+    <tableColumn id="40" xr3:uid="{D783CAA0-DB7C-4920-BE75-1BDD92D61C9D}" name="#던진공 차징3 튕겨내기 DPS4">
       <calculatedColumnFormula>( INDEX([1]!ProjectileTable[DirectDmg],MATCH([1]!CharacterTable[[#This Row],[DefaultBallDataId]],[1]!ProjectileTable[Index],0))+CharacterAtkTable[[#This Row],[ChargeProjectileDmg4]] )
 / ( CharacterAtkTable[[#This Row],[SwingCooldown]] + CharacterAtkTable[[#This Row],[ChargeTime3]] + CharacterAtkTable[[#This Row],[ThrowAfterDelay]])
 * (1 + (CharacterAtkTable[[#This Row],[ChargeBounceCount4]]/2))</calculatedColumnFormula>
@@ -911,14 +911,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5271B47-48F0-4BF6-A0D6-E5CF6B27B8C8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E191EC3E-4EAA-4FE3-AA36-CB97942B5779}">
   <sheetPr codeName="Sheet4">
     <tabColor theme="5" tint="0.79998168889431442"/>
   </sheetPr>
   <dimension ref="B1:AO3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>

</xml_diff>